<commit_message>
"Import Excel" educator list
</commit_message>
<xml_diff>
--- a/public/file/primer.xlsx
+++ b/public/file/primer.xlsx
@@ -11,7 +11,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+  <si>
+    <t>Ime i prezime</t>
+  </si>
+  <si>
+    <t>Grad</t>
+  </si>
+  <si>
+    <t>Broj računa</t>
+  </si>
+  <si>
+    <t>Cifra</t>
+  </si>
   <si>
     <t>Nikola Janković</t>
   </si>
@@ -53,10 +65,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -66,12 +84,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,11 +104,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -303,8 +330,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.75"/>
-    <col customWidth="1" min="2" max="2" width="18.38"/>
+    <col customWidth="1" min="1" max="1" width="18.0"/>
+    <col customWidth="1" min="2" max="2" width="12.38"/>
+    <col customWidth="1" min="3" max="3" width="17.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -317,63 +345,77 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2">
         <v>65000.0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1">
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2">
         <v>30000.0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1">
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2">
         <v>45000.0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45000.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1">
-        <v>45000.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1">
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2">
         <v>45000.0</v>
       </c>
     </row>

</xml_diff>